<commit_message>
Added images and 3 good templates
</commit_message>
<xml_diff>
--- a/TestData/Perfect minutiae/Normal fingers/Ale1439794734-Hamster-1-1.xlsx
+++ b/TestData/Perfect minutiae/Normal fingers/Ale1439794734-Hamster-1-1.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Users\dan\5. Research, Grants &amp; Competitions\Biometrics research\External and internal reports\RedGate Down Tools Week\Minutiae tagging\Ale1439794734\Enrolment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ag720\Desktop\Tagged minutiae\libAFIS\TestData\Perfect minutiae\Normal fingers\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13545" windowHeight="5700"/>
   </bookViews>
   <sheets>
     <sheet name="Ale1439794734-Hamster-1-1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
   <si>
     <t>X</t>
   </si>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -617,9 +620,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -652,9 +655,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -834,471 +837,516 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="A1:D33"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>135.91800000000001</v>
+        <v>71.429000000000002</v>
       </c>
       <c r="C2">
-        <v>11.429</v>
+        <v>47.347000000000001</v>
       </c>
       <c r="D2">
-        <v>143.74600000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>201.251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>181.63300000000001</v>
+        <v>115.91800000000001</v>
       </c>
       <c r="C3">
-        <v>59.591999999999999</v>
+        <v>60</v>
       </c>
       <c r="D3">
-        <v>145.00800000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>352.23500000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>113.06100000000001</v>
+        <v>182.857</v>
       </c>
       <c r="C4">
-        <v>23.265000000000001</v>
+        <v>61.633000000000003</v>
       </c>
       <c r="D4">
-        <v>152.10300000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>524.93200000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>118.776</v>
+        <v>49.387999999999998</v>
       </c>
       <c r="C5">
-        <v>52.652999999999999</v>
+        <v>94.694000000000003</v>
       </c>
       <c r="D5">
-        <v>154.654</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>209.05500000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>160</v>
+        <v>135.51</v>
       </c>
       <c r="C6">
-        <v>75.918000000000006</v>
+        <v>93.468999999999994</v>
       </c>
       <c r="D6">
-        <v>319.08600000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>177.614</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>143</v>
+        <v>93.061000000000007</v>
       </c>
       <c r="C7">
-        <v>91</v>
+        <v>102.857</v>
       </c>
       <c r="D7">
-        <v>137.291</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <v>11.31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>90</v>
+        <v>55.51</v>
       </c>
       <c r="C8">
-        <v>97</v>
+        <v>119.184</v>
       </c>
       <c r="D8">
-        <v>157.62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <v>210.06899999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>65</v>
+        <v>69.796000000000006</v>
       </c>
       <c r="C9">
-        <v>101</v>
+        <v>143.673</v>
       </c>
       <c r="D9">
-        <v>354.56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>9.4619999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>125</v>
+        <v>38.776000000000003</v>
       </c>
       <c r="C10">
-        <v>130</v>
+        <v>164.898</v>
       </c>
       <c r="D10">
-        <v>145.49100000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>53.061</v>
+        <v>84.897999999999996</v>
       </c>
       <c r="C11">
-        <v>117.551</v>
+        <v>165.30600000000001</v>
       </c>
       <c r="D11">
-        <v>189.46199999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>204.22800000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>170.20400000000001</v>
+        <v>195.91800000000001</v>
       </c>
       <c r="C12">
-        <v>169.79599999999999</v>
+        <v>164.08199999999999</v>
       </c>
       <c r="D12">
-        <v>310.91399999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+        <v>324.16199999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>107.34699999999999</v>
+        <v>161.63300000000001</v>
       </c>
       <c r="C13">
-        <v>160</v>
+        <v>172.245</v>
       </c>
       <c r="D13">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+        <v>341.565</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>92.245000000000005</v>
+        <v>181.63300000000001</v>
       </c>
       <c r="C14">
-        <v>149.79599999999999</v>
+        <v>180.816</v>
       </c>
       <c r="D14">
-        <v>159.14599999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+        <v>159.44399999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>69.796000000000006</v>
+        <v>57.143000000000001</v>
       </c>
       <c r="C15">
-        <v>147.34700000000001</v>
+        <v>189.79599999999999</v>
       </c>
       <c r="D15">
-        <v>344.745</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+        <v>40.914000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>44.082000000000001</v>
+        <v>167.755</v>
       </c>
       <c r="C16">
-        <v>192.245</v>
+        <v>203.26499999999999</v>
       </c>
       <c r="D16">
-        <v>217.56899999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>334.654</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>156.73500000000001</v>
+        <v>220.816</v>
       </c>
       <c r="C17">
-        <v>243.26499999999999</v>
+        <v>233.06100000000001</v>
       </c>
       <c r="D17">
-        <v>124.38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+        <v>147.995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>54.286000000000001</v>
+        <v>171.429</v>
       </c>
       <c r="C18">
-        <v>206.53100000000001</v>
+        <v>223.673</v>
       </c>
       <c r="D18">
-        <v>28.071999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+        <v>158.749</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>70.611999999999995</v>
+        <v>144.898</v>
       </c>
       <c r="C19">
-        <v>219.59200000000001</v>
+        <v>230.61199999999999</v>
       </c>
       <c r="D19">
-        <v>319.76400000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+        <v>341.565</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>45.305999999999997</v>
+        <v>89.796000000000006</v>
       </c>
       <c r="C20">
-        <v>229.38800000000001</v>
+        <v>222.041</v>
       </c>
       <c r="D20">
-        <v>28.071999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+        <v>208.072</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>102.041</v>
+        <v>69.796000000000006</v>
       </c>
       <c r="C21">
-        <v>244.898</v>
+        <v>233.46899999999999</v>
       </c>
       <c r="D21">
-        <v>127.569</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+        <v>37.569000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>175.102</v>
+        <v>46.122</v>
       </c>
       <c r="C22">
-        <v>286.53100000000001</v>
+        <v>258.77600000000001</v>
       </c>
       <c r="D22">
-        <v>142.595</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+        <v>243.435</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>150.61199999999999</v>
+        <v>102.041</v>
       </c>
       <c r="C23">
-        <v>282.44900000000001</v>
+        <v>240.816</v>
       </c>
       <c r="D23">
-        <v>137.12100000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+        <v>21.800999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>85.305999999999997</v>
+        <v>140</v>
       </c>
       <c r="C24">
-        <v>264.49</v>
+        <v>237.143</v>
       </c>
       <c r="D24">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>162.44900000000001</v>
+        <v>178.77600000000001</v>
       </c>
       <c r="C25">
-        <v>315.10199999999998</v>
+        <v>248.16300000000001</v>
       </c>
       <c r="D25">
-        <v>159.14599999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+        <v>323.13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
-        <v>81.224000000000004</v>
+        <v>197.959</v>
       </c>
       <c r="C26">
-        <v>268.16300000000001</v>
+        <v>269.79599999999999</v>
       </c>
       <c r="D26">
-        <v>292.38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+        <v>308.65999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
-        <v>55.51</v>
+        <v>132.245</v>
       </c>
       <c r="C27">
-        <v>266.12200000000001</v>
+        <v>251.429</v>
       </c>
       <c r="D27">
-        <v>243.435</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+        <v>340.71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
-        <v>72.245000000000005</v>
+        <v>155.91800000000001</v>
       </c>
       <c r="C28">
-        <v>260</v>
+        <v>271.02</v>
       </c>
       <c r="D28">
-        <v>282.529</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+        <v>145.49100000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>122.857</v>
+        <v>47.755000000000003</v>
       </c>
       <c r="C29">
-        <v>315.10199999999998</v>
+        <v>311.02</v>
       </c>
       <c r="D29">
-        <v>169.21600000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+        <v>56.31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
-        <v>106.122</v>
+        <v>87.754999999999995</v>
       </c>
       <c r="C30">
-        <v>304.49</v>
+        <v>283.673</v>
       </c>
       <c r="D30">
-        <v>164.476</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+        <v>35.537999999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
-        <v>167.34700000000001</v>
+        <v>164.08199999999999</v>
       </c>
       <c r="C31">
-        <v>337.959</v>
+        <v>325.714</v>
       </c>
       <c r="D31">
-        <v>168.69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+        <v>129.47200000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32">
-        <v>93.468999999999994</v>
+        <v>107.755</v>
       </c>
       <c r="C32">
-        <v>351.02</v>
+        <v>300.81599999999997</v>
       </c>
       <c r="D32">
-        <v>17.649999999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+        <v>348.11099999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
-        <v>153.06100000000001</v>
+        <v>43.265000000000001</v>
       </c>
       <c r="C33">
-        <v>359.59199999999998</v>
+        <v>350.61200000000002</v>
       </c>
       <c r="D33">
-        <v>182.726</v>
+        <v>56.31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>247.755</v>
+      </c>
+      <c r="C34">
+        <v>272.65300000000002</v>
+      </c>
+      <c r="D34">
+        <v>138.81399999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>209.38800000000001</v>
+      </c>
+      <c r="C35">
+        <v>371.02</v>
+      </c>
+      <c r="D35">
+        <v>154.44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>193.87799999999999</v>
+      </c>
+      <c r="C36">
+        <v>384.49</v>
+      </c>
+      <c r="D36">
+        <v>146.88900000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>